<commit_message>
maj_fichier script.js et création product.js
Mise à jour du code JS du fichier script.js.
Création du fichier product.js avec insertion du code pour visualiser l'image, nom, description et prix d'un produit lors d'un clic sur la page index.html
</commit_message>
<xml_diff>
--- a/documentations/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/documentations/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BriceThibault_5_02112021\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD2EB7C-A4A8-4A86-A3CC-88E1396E779D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF65343-6CEF-43D1-8FB8-CD166A208772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -611,7 +611,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -690,7 +690,7 @@
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
@@ -699,105 +699,105 @@
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A8" s="12"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A9" s="12"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A10" s="12"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A11" s="12"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A12" s="12"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A13" s="12"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A14" s="12"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A15" s="12"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A16" s="12"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A17" s="12"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A18" s="12"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A19" s="12"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A20" s="12"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A21" s="12"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>

</xml_diff>